<commit_message>
modifying basic settings v1.5
</commit_message>
<xml_diff>
--- a/runner/SBMS_AUTOTEST_RESULTS.xlsx
+++ b/runner/SBMS_AUTOTEST_RESULTS.xlsx
@@ -428,19 +428,19 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>39792666</v>
+        <v>39717666</v>
       </c>
       <c r="C1" t="n">
-        <v>39727666</v>
+        <v>39617666</v>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Было Katta Doimiy 100, Стало: Katta Doimiy 40</t>
+          <t>Было Katta Doimiy 40, Стало: Katta Doimiy 100</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>2024-10-23 22:18:29</t>
+          <t>2024-10-24 23:18:41</t>
         </is>
       </c>
     </row>

</xml_diff>